<commit_message>
GRAFICOS DIGAM SE FALTA ALGUMA COISA
</commit_message>
<xml_diff>
--- a/IPM.xlsx
+++ b/IPM.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D99F87-CC60-40E4-8B6E-66A0E6F785EB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BFD06C-5422-4ECC-8E3B-446C010206B1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{40B7943D-8E02-45B6-A0CC-5AF7CCF4F1F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Folha1!$P$5:$P$12</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Folha1!$Q$5:$Q$12</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="27">
   <si>
     <t>Tarefa 1</t>
   </si>
@@ -83,12 +87,36 @@
   <si>
     <t>tamanho da amostra</t>
   </si>
+  <si>
+    <t>]10;20[</t>
+  </si>
+  <si>
+    <t>[20;30[</t>
+  </si>
+  <si>
+    <t>[30;40[</t>
+  </si>
+  <si>
+    <t>[40;50[</t>
+  </si>
+  <si>
+    <t>[50;60[</t>
+  </si>
+  <si>
+    <t>[60;70[</t>
+  </si>
+  <si>
+    <t>[70;80[</t>
+  </si>
+  <si>
+    <t>[80;INF[</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +133,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -193,12 +226,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -212,6 +239,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -227,6 +256,2715 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Tarefa</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> 1- Tempo</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Folha1!$P$5:$P$12</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>]10;20[</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[20;30[</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>[30;40[</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>[40;50[</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>[50;60[</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>[60;70[</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>[70;80[</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>[80;INF[</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$Q$5:$Q$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E4B2-40C2-A543-6C557DFB0834}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="544497944"/>
+        <c:axId val="544500240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="544497944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544500240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="544500240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="544497944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Tarefa</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> 2- Tempo</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$S$5:$S$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$S$5:$S$8</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>]10;20[</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[20;30[</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>[30;40[</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>[40;50[</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$T$5:$T$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$T$5:$T$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F989-4633-99D0-680E3332F30C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="605874304"/>
+        <c:axId val="605879880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="605874304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="605879880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="605879880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="605874304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$V$5:$V$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$V$5:$V$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>]10;20[</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>[20;30[</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>[30;40[</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>[40;50[</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>[50;60[</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Folha1!$W$5:$W$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Folha1!$W$5:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B5A2-4FC0-AEC5-1CCD96244A07}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="570827808"/>
+        <c:axId val="605875616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="570827808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="605875616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="605875616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="570827808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47795672-C596-42F2-91F2-CCFB7989AEFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26ED9E61-BD70-44A3-A6F8-DA6477EBF703}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5146134-0570-4E80-BB2F-C8B05971FF6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,10 +3264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC247D32-A791-4790-8217-EFE3184E390B}">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" topLeftCell="P29" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +3287,7 @@
     <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -571,7 +3309,7 @@
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -615,7 +3353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -628,7 +3366,7 @@
       <c r="D3" s="6">
         <v>3</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>118</v>
       </c>
       <c r="F3" s="6">
@@ -640,7 +3378,7 @@
       <c r="H3" s="6">
         <v>0</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="9">
         <v>29</v>
       </c>
       <c r="J3" s="6">
@@ -652,15 +3390,14 @@
       <c r="L3" s="6">
         <v>0</v>
       </c>
-      <c r="M3" s="9">
+      <c r="M3" s="7">
         <v>29</v>
       </c>
       <c r="N3" s="6">
         <v>5</v>
       </c>
-      <c r="Q3" s="7"/>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -673,7 +3410,7 @@
       <c r="D4" s="6">
         <v>3</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>59</v>
       </c>
       <c r="F4" s="6">
@@ -685,7 +3422,7 @@
       <c r="H4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="9">
         <v>38</v>
       </c>
       <c r="J4" s="6">
@@ -697,15 +3434,26 @@
       <c r="L4" s="6">
         <v>0</v>
       </c>
-      <c r="M4" s="9">
+      <c r="M4" s="7">
         <v>34</v>
       </c>
       <c r="N4" s="6">
         <v>5</v>
       </c>
-      <c r="Q4" s="7"/>
+      <c r="P4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="12"/>
+      <c r="S4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" s="12"/>
+      <c r="V4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="W4" s="12"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -718,7 +3466,7 @@
       <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="9">
         <v>35</v>
       </c>
       <c r="F5" s="6">
@@ -730,7 +3478,7 @@
       <c r="H5" s="6">
         <v>0</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="9">
         <v>30</v>
       </c>
       <c r="J5" s="6">
@@ -742,15 +3490,32 @@
       <c r="L5" s="6">
         <v>0</v>
       </c>
-      <c r="M5" s="9">
+      <c r="M5" s="7">
         <v>24</v>
       </c>
       <c r="N5" s="6">
         <v>5</v>
       </c>
-      <c r="Q5" s="7"/>
+      <c r="P5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>0</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="13">
+        <v>3</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="W5" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -763,7 +3528,7 @@
       <c r="D6" s="6">
         <v>3</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>36</v>
       </c>
       <c r="F6" s="6">
@@ -775,7 +3540,7 @@
       <c r="H6" s="6">
         <v>0</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>21</v>
       </c>
       <c r="J6" s="6">
@@ -787,15 +3552,32 @@
       <c r="L6" s="6">
         <v>0</v>
       </c>
-      <c r="M6" s="9">
+      <c r="M6" s="7">
         <v>25</v>
       </c>
       <c r="N6" s="6">
         <v>5</v>
       </c>
-      <c r="Q6" s="7"/>
+      <c r="P6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>2</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="13">
+        <v>10</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W6" s="13">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -808,7 +3590,7 @@
       <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>33</v>
       </c>
       <c r="F7" s="1">
@@ -820,7 +3602,7 @@
       <c r="H7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="10">
         <v>20</v>
       </c>
       <c r="J7" s="1">
@@ -832,15 +3614,32 @@
       <c r="L7" s="1">
         <v>0</v>
       </c>
-      <c r="M7" s="9">
+      <c r="M7" s="7">
         <v>23</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="7">
         <v>5</v>
       </c>
-      <c r="Q7" s="8"/>
+      <c r="P7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>8</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="13">
+        <v>2</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W7" s="13">
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -853,7 +3652,7 @@
       <c r="D8" s="1">
         <v>2</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>30</v>
       </c>
       <c r="F8" s="1">
@@ -865,7 +3664,7 @@
       <c r="H8" s="1">
         <v>0</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="10">
         <v>26</v>
       </c>
       <c r="J8" s="1">
@@ -877,15 +3676,32 @@
       <c r="L8" s="1">
         <v>0</v>
       </c>
-      <c r="M8" s="9">
+      <c r="M8" s="7">
         <v>50</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="7">
         <v>5</v>
       </c>
-      <c r="Q8" s="8"/>
+      <c r="P8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>1</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8" s="13">
+        <v>0</v>
+      </c>
+      <c r="V8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="W8" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
@@ -898,7 +3714,7 @@
       <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>27</v>
       </c>
       <c r="F9" s="1">
@@ -910,7 +3726,7 @@
       <c r="H9" s="1">
         <v>0</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="10">
         <v>21</v>
       </c>
       <c r="J9" s="1">
@@ -922,15 +3738,32 @@
       <c r="L9" s="1">
         <v>0</v>
       </c>
-      <c r="M9" s="9">
+      <c r="M9" s="7">
         <v>37</v>
       </c>
-      <c r="N9" s="9">
+      <c r="N9" s="7">
         <v>5</v>
       </c>
-      <c r="Q9" s="8"/>
+      <c r="P9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q9" s="13">
+        <v>2</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" s="13">
+        <v>0</v>
+      </c>
+      <c r="V9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="W9" s="13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -943,7 +3776,7 @@
       <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>47</v>
       </c>
       <c r="F10" s="1">
@@ -955,7 +3788,7 @@
       <c r="H10" s="1">
         <v>1</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="10">
         <v>28</v>
       </c>
       <c r="J10" s="1">
@@ -967,15 +3800,32 @@
       <c r="L10" s="1">
         <v>0</v>
       </c>
-      <c r="M10" s="9">
+      <c r="M10" s="7">
         <v>25</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="7">
         <v>5</v>
       </c>
-      <c r="Q10" s="8"/>
+      <c r="P10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="13">
+        <v>0</v>
+      </c>
+      <c r="S10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="T10" s="13">
+        <v>0</v>
+      </c>
+      <c r="V10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="W10" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -988,7 +3838,7 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>37</v>
       </c>
       <c r="F11" s="1">
@@ -1000,7 +3850,7 @@
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="10">
         <v>19</v>
       </c>
       <c r="J11" s="1">
@@ -1012,15 +3862,32 @@
       <c r="L11" s="1">
         <v>0</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="7">
         <v>21</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="7">
         <v>4</v>
       </c>
-      <c r="Q11" s="8"/>
+      <c r="P11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="13">
+        <v>1</v>
+      </c>
+      <c r="S11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T11" s="13">
+        <v>0</v>
+      </c>
+      <c r="V11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="W11" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -1033,7 +3900,7 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <v>51</v>
       </c>
       <c r="F12" s="1">
@@ -1045,7 +3912,7 @@
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="10">
         <v>24</v>
       </c>
       <c r="J12" s="1">
@@ -1057,15 +3924,32 @@
       <c r="L12" s="1">
         <v>1</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="7">
         <v>20</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="7">
         <v>5</v>
       </c>
-      <c r="Q12" s="8"/>
+      <c r="P12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="13">
+        <v>1</v>
+      </c>
+      <c r="S12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="T12" s="13">
+        <v>0</v>
+      </c>
+      <c r="V12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="W12" s="13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
@@ -1078,7 +3962,7 @@
       <c r="D13" s="1">
         <v>3</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <v>72</v>
       </c>
       <c r="F13" s="1">
@@ -1090,7 +3974,7 @@
       <c r="H13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="10">
         <v>25</v>
       </c>
       <c r="J13" s="1">
@@ -1102,15 +3986,29 @@
       <c r="L13" s="1">
         <v>0</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="7">
         <v>32</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="7">
         <v>5</v>
       </c>
-      <c r="Q13" s="8"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="10">
+        <f>SUM(Q5:Q12)</f>
+        <v>15</v>
+      </c>
+      <c r="S13" s="12"/>
+      <c r="T13" s="13">
+        <f>SUM(T5:T12)</f>
+        <v>15</v>
+      </c>
+      <c r="V13" s="12"/>
+      <c r="W13" s="13">
+        <f>SUM(W5:W12)</f>
+        <v>15</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -1123,7 +4021,7 @@
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="10">
         <v>26</v>
       </c>
       <c r="F14" s="1">
@@ -1135,7 +4033,7 @@
       <c r="H14" s="1">
         <v>0</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="10">
         <v>16</v>
       </c>
       <c r="J14" s="1">
@@ -1147,15 +4045,14 @@
       <c r="L14" s="1">
         <v>0</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="7">
         <v>28</v>
       </c>
-      <c r="N14" s="9">
+      <c r="N14" s="7">
         <v>5</v>
       </c>
-      <c r="Q14" s="8"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -1168,7 +4065,7 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="10">
         <v>39</v>
       </c>
       <c r="F15" s="1">
@@ -1180,7 +4077,7 @@
       <c r="H15" s="1">
         <v>0</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="10">
         <v>22</v>
       </c>
       <c r="J15" s="1">
@@ -1192,15 +4089,15 @@
       <c r="L15" s="1">
         <v>0</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="7">
         <v>22</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="7">
         <v>5</v>
       </c>
-      <c r="Q15" s="8"/>
+      <c r="Q15" s="10"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
@@ -1213,7 +4110,7 @@
       <c r="D16" s="1">
         <v>3</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="10">
         <v>33</v>
       </c>
       <c r="F16" s="1">
@@ -1225,7 +4122,7 @@
       <c r="H16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="10">
         <v>13</v>
       </c>
       <c r="J16" s="1">
@@ -1237,13 +4134,13 @@
       <c r="L16" s="1">
         <v>0</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="7">
         <v>22</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="7">
         <v>5</v>
       </c>
-      <c r="Q16" s="8"/>
+      <c r="Q16" s="10"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
@@ -1258,7 +4155,7 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="10">
         <v>30</v>
       </c>
       <c r="F17" s="1">
@@ -1270,7 +4167,7 @@
       <c r="H17" s="1">
         <v>0</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="10">
         <v>29</v>
       </c>
       <c r="J17" s="1">
@@ -1279,31 +4176,41 @@
       <c r="K17" s="1">
         <v>13</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="8">
         <v>1</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M17" s="7">
         <v>26</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="7">
         <v>5</v>
       </c>
-      <c r="Q17" s="8"/>
+      <c r="Q17" s="10"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <f>13/15*100</f>
+        <v>86.666666666666671</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1">
+        <f>3/15*100</f>
+        <v>20</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
+      <c r="L18" s="1">
+        <f>2/15*100</f>
+        <v>13.333333333333334</v>
+      </c>
       <c r="M18" s="1"/>
+      <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
@@ -1393,7 +4300,7 @@
       <c r="H22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="10">
         <f>AVERAGE(E3:E17)</f>
         <v>44.866666666666667</v>
       </c>
@@ -1551,7 +4458,7 @@
       <c r="M27" s="1"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I29" s="13"/>
+      <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
@@ -1570,7 +4477,7 @@
       <c r="H30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I30" s="12"/>
+      <c r="I30" s="10"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1" t="s">
         <v>8</v>
@@ -1599,7 +4506,7 @@
       <c r="H31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="12">
+      <c r="I31" s="10">
         <f>AVERAGE(I3:I17)</f>
         <v>24.066666666666666</v>
       </c>
@@ -1634,7 +4541,7 @@
       <c r="H32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="10">
         <f>_xlfn.STDEV.S(I3:I17)</f>
         <v>6.2731476112379889</v>
       </c>
@@ -1663,7 +4570,7 @@
       <c r="H33" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I33" s="12"/>
+      <c r="I33" s="10"/>
       <c r="J33" s="1"/>
       <c r="K33" s="5" t="s">
         <v>14</v>
@@ -1742,10 +4649,10 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I37" s="13"/>
+      <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I38" s="13"/>
+      <c r="I38" s="11"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
@@ -1764,7 +4671,7 @@
       <c r="H39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="12"/>
+      <c r="I39" s="10"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="s">
         <v>8</v>
@@ -1793,7 +4700,7 @@
       <c r="H40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40" s="10">
         <f>AVERAGE(M3:M17)</f>
         <v>27.866666666666667</v>
       </c>
@@ -1828,7 +4735,7 @@
       <c r="H41" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="12">
+      <c r="I41" s="10">
         <f>_xlfn.STDEV.S(M3:M17)</f>
         <v>7.8637201907300378</v>
       </c>
@@ -1857,7 +4764,7 @@
       <c r="H42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I42" s="12"/>
+      <c r="I42" s="10"/>
       <c r="J42" s="1"/>
       <c r="K42" s="5" t="s">
         <v>14</v>
@@ -1880,7 +4787,7 @@
       <c r="H43" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I43" s="12"/>
+      <c r="I43" s="10"/>
       <c r="J43" s="1"/>
       <c r="K43" s="5" t="s">
         <v>15</v>
@@ -1938,5 +4845,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>